<commit_message>
Experimentos y resultados preliminares.
</commit_message>
<xml_diff>
--- a/Resultados240816_11_53.xlsx
+++ b/Resultados240816_11_53.xlsx
@@ -2,25 +2,26 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerardo\Dropbox\INGENIERIA\ENSAYO COMETA\matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9855" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="1" r:id="rId1"/>
     <sheet name="Grafica" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="28">
   <si>
     <t>0309120ctol.bmp</t>
   </si>
@@ -93,11 +94,23 @@
   <si>
     <t xml:space="preserve">K-Means </t>
   </si>
+  <si>
+    <t>Validacion ANOVA</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Area Halo</t>
+  </si>
+  <si>
+    <t>Area Cola</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -144,11 +157,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -160,10 +182,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -182,7 +210,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -349,7 +377,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-F91D-4C41-A706-33D3E0C643D0}"/>
             </c:ext>
@@ -442,14 +470,13 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000005-F91D-4C41-A706-33D3E0C643D0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -458,11 +485,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1078658143"/>
-        <c:axId val="1078658559"/>
+        <c:axId val="259359768"/>
+        <c:axId val="203879904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1078658143"/>
+        <c:axId val="259359768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -504,7 +531,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078658559"/>
+        <c:crossAx val="203879904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -512,7 +539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1078658559"/>
+        <c:axId val="203879904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,7 +646,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078658143"/>
+        <c:crossAx val="259359768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -708,7 +735,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -878,7 +905,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-BBD7-460C-9BAA-06474BDE7639}"/>
             </c:ext>
@@ -971,7 +998,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-BBD7-460C-9BAA-06474BDE7639}"/>
             </c:ext>
@@ -986,11 +1013,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1078658143"/>
-        <c:axId val="1078658559"/>
+        <c:axId val="203883432"/>
+        <c:axId val="203881864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1078658143"/>
+        <c:axId val="203883432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1059,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078658559"/>
+        <c:crossAx val="203881864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1040,7 +1067,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1078658559"/>
+        <c:axId val="203881864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,7 +1174,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078658143"/>
+        <c:crossAx val="203883432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1236,7 +1263,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1398,7 +1425,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-FC2C-4868-810A-3FC578EFFF36}"/>
             </c:ext>
@@ -1491,7 +1518,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-FC2C-4868-810A-3FC578EFFF36}"/>
             </c:ext>
@@ -1506,11 +1533,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1078658143"/>
-        <c:axId val="1078658559"/>
+        <c:axId val="203881472"/>
+        <c:axId val="259208080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1078658143"/>
+        <c:axId val="203881472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1552,7 +1579,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078658559"/>
+        <c:crossAx val="259208080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1560,7 +1587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1078658559"/>
+        <c:axId val="259208080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,7 +1694,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078658143"/>
+        <c:crossAx val="203881472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1756,7 +1783,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1918,7 +1945,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-40AF-4F83-906A-E96A40F7956B}"/>
             </c:ext>
@@ -2011,7 +2038,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-40AF-4F83-906A-E96A40F7956B}"/>
             </c:ext>
@@ -2026,11 +2053,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1078658143"/>
-        <c:axId val="1078658559"/>
+        <c:axId val="259205336"/>
+        <c:axId val="259207296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1078658143"/>
+        <c:axId val="259205336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2072,7 +2099,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078658559"/>
+        <c:crossAx val="259207296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2080,7 +2107,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1078658559"/>
+        <c:axId val="259207296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2187,7 +2214,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078658143"/>
+        <c:crossAx val="259205336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4895,36 +4922,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B36"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -5904,29 +5931,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T44" sqref="T44"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -5950,10 +5977,10 @@
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -5975,10 +6002,10 @@
       <c r="G3" s="1">
         <v>0.32290412936791718</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -6000,10 +6027,10 @@
       <c r="G4" s="1">
         <v>0.45803650678536439</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -6025,10 +6052,10 @@
       <c r="G5" s="1">
         <v>0.43074876176746063</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -6050,10 +6077,10 @@
       <c r="G6" s="1">
         <v>2.0467695872606964</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -6075,10 +6102,10 @@
       <c r="G7" s="1">
         <v>0.28376819131191028</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -6100,10 +6127,10 @@
       <c r="G8" s="1">
         <v>0.49492327401739578</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -6125,10 +6152,10 @@
       <c r="G9" s="1">
         <v>0.38481959638538132</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -6150,10 +6177,10 @@
       <c r="G10" s="1">
         <v>0.27066667983254467</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -6175,10 +6202,10 @@
       <c r="G11" s="1">
         <v>0.42596479371080637</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -6200,10 +6227,10 @@
       <c r="G12" s="1">
         <v>0.61879224281097345</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -6225,10 +6252,10 @@
       <c r="G13" s="1">
         <v>1.2115921167111199</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
@@ -6250,10 +6277,10 @@
       <c r="G14" s="1">
         <v>0.52816967598408537</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -6275,10 +6302,10 @@
       <c r="G15" s="1">
         <v>0.92821049020586677</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -6300,10 +6327,10 @@
       <c r="G16" s="1">
         <v>1.0542225713618016</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -6325,10 +6352,10 @@
       <c r="G17" s="1">
         <v>2.7338777423883855</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -6350,10 +6377,10 @@
       <c r="G18" s="1">
         <v>2.9743225150045296</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -6375,48 +6402,48 @@
       <c r="G19" s="1">
         <v>3.0208298818618453</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G20">
         <f>AVERAGE(G3:G19)</f>
         <v>1.0699187503981225</v>
       </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="6"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -6844,4 +6871,527 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="J2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2938</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2951</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2134</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2033</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4823</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4487</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.32290412936791718</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.24981924346670734</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3218</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3299</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2008</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1955</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5111</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4858</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.45803650678536439</v>
+      </c>
+      <c r="K5" s="1">
+        <v>9.6428719022243384E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3169</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3208</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2269</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2184</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5005</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4800</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.43074876176746063</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.11658311819922973</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1639</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1743</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4936</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4773</v>
+      </c>
+      <c r="G7" s="1">
+        <v>22055</v>
+      </c>
+      <c r="H7" s="1">
+        <v>19162</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2.0467695872606964</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.37982058565482507</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5160</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5213</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3129</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4428</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4166</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.28376819131191028</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.15993652583931559</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4896</v>
+      </c>
+      <c r="B9" s="1">
+        <v>4899</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2860</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2739</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4649</v>
+      </c>
+      <c r="H9" s="1">
+        <v>4412</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.49492327401739578</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.10097899274450407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>5721</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5774</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2707</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2596</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3890</v>
+      </c>
+      <c r="H10" s="1">
+        <v>3572</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.38481959638538132</v>
+      </c>
+      <c r="K10" s="1">
+        <v>8.3447163320156489E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>5545</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5551</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3337</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3215</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3773</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3521</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.27066667983254467</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.10877099820395481</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>6300</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6301</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2780</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2678</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4246</v>
+      </c>
+      <c r="H12" s="1">
+        <v>3955</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.42596479371080637</v>
+      </c>
+      <c r="K12" s="1">
+        <v>5.9416144511602612E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>6619</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6637</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2980</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2851</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4458</v>
+      </c>
+      <c r="H13" s="1">
+        <v>4051</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.61879224281097345</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.10878855270794681</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>5228</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5147</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3838</v>
+      </c>
+      <c r="E14" s="1">
+        <v>3574</v>
+      </c>
+      <c r="G14" s="1">
+        <v>8294</v>
+      </c>
+      <c r="H14" s="1">
+        <v>7020</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.2115921167111199</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.22143397623047015</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>5089</v>
+      </c>
+      <c r="B15" s="1">
+        <v>5089</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3552</v>
+      </c>
+      <c r="E15" s="1">
+        <v>3377</v>
+      </c>
+      <c r="G15" s="1">
+        <v>4729</v>
+      </c>
+      <c r="H15" s="1">
+        <v>4454</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.52816967598408537</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.13051517714871699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>5995</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6015</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3806</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3579</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5717</v>
+      </c>
+      <c r="H16" s="1">
+        <v>5173</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.92821049020586677</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.14045322072119024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>7645</v>
+      </c>
+      <c r="B17" s="1">
+        <v>7782</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5417</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5192</v>
+      </c>
+      <c r="G17" s="1">
+        <v>14878</v>
+      </c>
+      <c r="H17" s="1">
+        <v>13761</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1.0542225713618016</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.20300650138369722</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>4728</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4699</v>
+      </c>
+      <c r="D18" s="1">
+        <v>7556</v>
+      </c>
+      <c r="E18" s="1">
+        <v>6775</v>
+      </c>
+      <c r="G18" s="1">
+        <v>25718</v>
+      </c>
+      <c r="H18" s="1">
+        <v>21611</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2.7338777423883855</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.53997837138820648</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>3737</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3581</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7284</v>
+      </c>
+      <c r="E19" s="1">
+        <v>6010</v>
+      </c>
+      <c r="G19" s="1">
+        <v>32221</v>
+      </c>
+      <c r="H19" s="1">
+        <v>25143</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2.9743225150045296</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.60860477899428056</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1483</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1466</v>
+      </c>
+      <c r="D20" s="1">
+        <v>6663</v>
+      </c>
+      <c r="E20" s="1">
+        <v>5983</v>
+      </c>
+      <c r="G20" s="1">
+        <v>21906</v>
+      </c>
+      <c r="H20" s="1">
+        <v>18541</v>
+      </c>
+      <c r="J20" s="1">
+        <v>3.0208298818618453</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.55248376116951037</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>